<commit_message>
Sectioning and drawing keyboard init
</commit_message>
<xml_diff>
--- a/tests/unit/graphics/testFiles/GUI items placement.xlsx
+++ b/tests/unit/graphics/testFiles/GUI items placement.xlsx
@@ -217,10 +217,10 @@
     <t xml:space="preserve">capital_m_pushed</t>
   </si>
   <si>
-    <t xml:space="preserve">keyboard_capital_pushed </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Keyboard erase </t>
+    <t xml:space="preserve">keyboard_capital_pushed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keyboard erase</t>
   </si>
   <si>
     <t xml:space="preserve">Keyboard erase_pushed</t>
@@ -238,10 +238,10 @@
     <t xml:space="preserve">Keyboard_special_pushed</t>
   </si>
   <si>
-    <t xml:space="preserve">Keyboard space </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Keyboard space_pushed </t>
+    <t xml:space="preserve">Keyboard space</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keyboard space_pushed</t>
   </si>
   <si>
     <t xml:space="preserve">keyboard_lowcase</t>
@@ -403,7 +403,7 @@
     <t xml:space="preserve">lowcase_m_pushed</t>
   </si>
   <si>
-    <t xml:space="preserve">keyboard_lowcase_pushed </t>
+    <t xml:space="preserve">keyboard_lowcase_pushed</t>
   </si>
   <si>
     <t xml:space="preserve">keyboard_numbers</t>
@@ -565,10 +565,10 @@
     <t xml:space="preserve">Keyboard_s16_pushed</t>
   </si>
   <si>
-    <t xml:space="preserve">Keyboard_letters_left </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Keyboard_letters_left_pushed </t>
+    <t xml:space="preserve">Keyboard_letters_left</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keyboard_letters_left_pushed</t>
   </si>
   <si>
     <t xml:space="preserve">keyboard_Special</t>
@@ -1064,7 +1064,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>